<commit_message>
Unificamos el testing del sprint 1
</commit_message>
<xml_diff>
--- a/Testing/Testing PI local.xlsx
+++ b/Testing/Testing PI local.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dina\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1p3p\OneDrive\Documentos\PI\grupo-09\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA118F-1A69-4C53-8DD8-7FBE44CA74BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Prueba" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="247">
   <si>
     <t>ID</t>
   </si>
@@ -730,11 +731,68 @@
   <si>
     <t>TO DO</t>
   </si>
+  <si>
+    <t>CP-027</t>
+  </si>
+  <si>
+    <t>CP-028</t>
+  </si>
+  <si>
+    <t>Validar get en postman</t>
+  </si>
+  <si>
+    <t>Validar post en postman</t>
+  </si>
+  <si>
+    <t>Validar delete en postman</t>
+  </si>
+  <si>
+    <t>Llamar categorias en postan</t>
+  </si>
+  <si>
+    <t>Agregar una categoria en postan</t>
+  </si>
+  <si>
+    <t>Eliminar la categoria ageregada por el post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingresar a postman y traer un get para ver las categotias </t>
+  </si>
+  <si>
+    <t>[Ingresar datros con categoria nueva a postman</t>
+  </si>
+  <si>
+    <t>Ingresar id a eliminar en postman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 categorias </t>
+  </si>
+  <si>
+    <t>5 categorias</t>
+  </si>
+  <si>
+    <t>CP-029</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>visualizar categorias en postman creadas por back</t>
+  </si>
+  <si>
+    <t>agregar nueva categoria en la base de datos</t>
+  </si>
+  <si>
+    <t>eliminar categoria en la base de datos creadas anteriormente</t>
+  </si>
+  <si>
+    <t>visualizar categorias en la base de datos creadas por back</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -1049,19 +1107,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF073763"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF073763"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF073763"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right/>
@@ -1099,12 +1144,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF073763"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF073763"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1150,113 +1206,147 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1473,15 +1563,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z39"/>
+  <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1495,46 +1585,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="25" t="s">
+      <c r="H1" s="40"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="13.8">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1544,11 +1634,11 @@
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-    </row>
-    <row r="3" spans="1:13" ht="66">
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+    </row>
+    <row r="3" spans="1:13" ht="79.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1585,7 +1675,7 @@
       </c>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" ht="66">
+    <row r="4" spans="1:13" ht="79.2">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1808,7 +1898,7 @@
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" ht="109.8" customHeight="1">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="26" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="3">
@@ -1823,7 +1913,7 @@
       <c r="E10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="27" t="s">
         <v>225</v>
       </c>
       <c r="G10" s="5">
@@ -1836,8 +1926,8 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="92.4">
-      <c r="A11" s="63" t="s">
+    <row r="11" spans="1:13" ht="105.6">
+      <c r="A11" s="26" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="3">
@@ -1873,8 +1963,8 @@
       </c>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="92.4">
-      <c r="A12" s="63" t="s">
+    <row r="12" spans="1:13" ht="105.6">
+      <c r="A12" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="3">
@@ -1910,8 +2000,8 @@
       </c>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="92.4">
-      <c r="A13" s="63" t="s">
+    <row r="13" spans="1:13" ht="105.6">
+      <c r="A13" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B13" s="3">
@@ -1947,8 +2037,8 @@
       </c>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:13" ht="145.19999999999999">
-      <c r="A14" s="63" t="s">
+    <row r="14" spans="1:13" ht="158.4">
+      <c r="A14" s="26" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="3">
@@ -1985,7 +2075,7 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="132">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="26" t="s">
         <v>81</v>
       </c>
       <c r="B15" s="3">
@@ -2022,7 +2112,7 @@
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="92.4">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B16" s="3">
@@ -2059,7 +2149,7 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:26" ht="92.4">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="26" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="3">
@@ -2096,7 +2186,7 @@
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="93" thickBot="1">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="3">
@@ -2139,16 +2229,16 @@
       <c r="B19" s="10">
         <v>44779</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="28" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="9">
@@ -2185,10 +2275,10 @@
     <row r="20" spans="1:26" ht="13.8" thickBot="1">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
       <c r="G20" s="9"/>
       <c r="H20" s="11"/>
       <c r="I20" s="9"/>
@@ -2210,13 +2300,13 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
     </row>
-    <row r="21" spans="1:26" ht="53.4" thickBot="1">
+    <row r="21" spans="1:26" ht="66.599999999999994" thickBot="1">
       <c r="A21" s="12"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="9">
         <v>2</v>
       </c>
@@ -2255,16 +2345,16 @@
       <c r="B22" s="10">
         <v>44779</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="28" t="s">
         <v>138</v>
       </c>
       <c r="G22" s="9">
@@ -2273,7 +2363,7 @@
       <c r="H22" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="28" t="s">
         <v>140</v>
       </c>
       <c r="J22" s="12"/>
@@ -2297,17 +2387,17 @@
     <row r="23" spans="1:26" ht="40.200000000000003" thickBot="1">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
       <c r="G23" s="9">
         <v>2</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I23" s="22"/>
+      <c r="I23" s="29"/>
       <c r="J23" s="12"/>
       <c r="K23" s="9" t="s">
         <v>93</v>
@@ -2337,16 +2427,16 @@
       <c r="B24" s="10">
         <v>44779</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="34" t="s">
         <v>144</v>
       </c>
       <c r="G24" s="11">
@@ -2355,7 +2445,7 @@
       <c r="H24" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="34" t="s">
         <v>98</v>
       </c>
       <c r="J24" s="12"/>
@@ -2383,17 +2473,17 @@
     <row r="25" spans="1:26" ht="40.200000000000003" thickBot="1">
       <c r="A25" s="12"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
       <c r="G25" s="11">
         <v>2</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -2413,22 +2503,22 @@
       <c r="Z25" s="12"/>
     </row>
     <row r="26" spans="1:26" ht="40.200000000000003" thickBot="1">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="44">
         <v>44779</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="28" t="s">
         <v>95</v>
       </c>
       <c r="G26" s="9">
@@ -2437,7 +2527,7 @@
       <c r="H26" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="28" t="s">
         <v>148</v>
       </c>
       <c r="J26" s="12"/>
@@ -2463,19 +2553,19 @@
       <c r="Z26" s="13"/>
     </row>
     <row r="27" spans="1:26" ht="53.4" thickBot="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
       <c r="G27" s="9">
         <v>2</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="I27" s="22"/>
+      <c r="I27" s="29"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="9" t="s">
@@ -2497,22 +2587,22 @@
       <c r="Z27" s="13"/>
     </row>
     <row r="28" spans="1:26" ht="39.6" customHeight="1" thickBot="1">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="42">
         <v>44779</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="34" t="s">
         <v>105</v>
       </c>
       <c r="G28" s="11" t="s">
@@ -2521,14 +2611,14 @@
       <c r="H28" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="I28" s="17" t="s">
+      <c r="I28" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="21" t="s">
+      <c r="J28" s="34"/>
+      <c r="K28" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="21" t="s">
+      <c r="L28" s="28" t="s">
         <v>153</v>
       </c>
       <c r="M28" s="13"/>
@@ -2547,22 +2637,22 @@
       <c r="Z28" s="13"/>
     </row>
     <row r="29" spans="1:26" ht="40.200000000000003" thickBot="1">
-      <c r="A29" s="18"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
       <c r="G29" s="11" t="s">
         <v>154</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
@@ -2579,22 +2669,22 @@
       <c r="Z29" s="13"/>
     </row>
     <row r="30" spans="1:26" ht="72" customHeight="1" thickBot="1">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="23">
+      <c r="B30" s="44">
         <v>44779</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="28" t="s">
         <v>157</v>
       </c>
       <c r="G30" s="9">
@@ -2603,14 +2693,14 @@
       <c r="H30" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="I30" s="21" t="s">
+      <c r="I30" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21" t="s">
+      <c r="J30" s="28"/>
+      <c r="K30" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="L30" s="21" t="s">
+      <c r="L30" s="28" t="s">
         <v>133</v>
       </c>
       <c r="M30" s="13"/>
@@ -2629,22 +2719,22 @@
       <c r="Z30" s="13"/>
     </row>
     <row r="31" spans="1:26" ht="72.75" customHeight="1" thickBot="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
       <c r="G31" s="9">
         <v>2</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
@@ -2661,22 +2751,22 @@
       <c r="Z31" s="13"/>
     </row>
     <row r="32" spans="1:26" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="44">
         <v>44779</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="28" t="s">
         <v>111</v>
       </c>
       <c r="G32" s="9" t="s">
@@ -2685,14 +2775,14 @@
       <c r="H32" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="I32" s="21" t="s">
+      <c r="I32" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21" t="s">
+      <c r="J32" s="28"/>
+      <c r="K32" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="L32" s="21" t="s">
+      <c r="L32" s="28" t="s">
         <v>133</v>
       </c>
       <c r="M32" s="13"/>
@@ -2711,22 +2801,22 @@
       <c r="Z32" s="13"/>
     </row>
     <row r="33" spans="1:26" ht="79.8" thickBot="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
       <c r="G33" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
@@ -2743,22 +2833,22 @@
       <c r="Z33" s="13"/>
     </row>
     <row r="34" spans="1:26" ht="26.4" customHeight="1" thickBot="1">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="42">
         <v>44779</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="34" t="s">
         <v>115</v>
       </c>
       <c r="G34" s="11">
@@ -2767,14 +2857,14 @@
       <c r="H34" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="I34" s="17" t="s">
+      <c r="I34" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="J34" s="17"/>
-      <c r="K34" s="21" t="s">
+      <c r="J34" s="34"/>
+      <c r="K34" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="L34" s="21" t="s">
+      <c r="L34" s="28" t="s">
         <v>153</v>
       </c>
       <c r="M34" s="13"/>
@@ -2793,22 +2883,22 @@
       <c r="Z34" s="13"/>
     </row>
     <row r="35" spans="1:26" ht="66.599999999999994" thickBot="1">
-      <c r="A35" s="18"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
       <c r="G35" s="11">
         <v>2</v>
       </c>
       <c r="H35" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
@@ -2825,22 +2915,22 @@
       <c r="Z35" s="13"/>
     </row>
     <row r="36" spans="1:26" ht="66" customHeight="1" thickBot="1">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B36" s="42">
         <v>44779</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="34" t="s">
         <v>168</v>
       </c>
       <c r="G36" s="11">
@@ -2849,14 +2939,14 @@
       <c r="H36" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="I36" s="17" t="s">
+      <c r="I36" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="J36" s="17"/>
-      <c r="K36" s="21" t="s">
+      <c r="J36" s="34"/>
+      <c r="K36" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="L36" s="21" t="s">
+      <c r="L36" s="28" t="s">
         <v>133</v>
       </c>
       <c r="M36" s="13"/>
@@ -2875,22 +2965,22 @@
       <c r="Z36" s="13"/>
     </row>
     <row r="37" spans="1:26" ht="53.4" thickBot="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
       <c r="G37" s="11">
         <v>2</v>
       </c>
       <c r="H37" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
       <c r="O37" s="13"/>
@@ -2907,22 +2997,22 @@
       <c r="Z37" s="13"/>
     </row>
     <row r="38" spans="1:26" ht="53.4" customHeight="1">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="B38" s="34">
+      <c r="B38" s="32">
         <v>44779</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="E38" s="32" t="s">
+      <c r="E38" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="30" t="s">
         <v>161</v>
       </c>
       <c r="G38" s="15">
@@ -2931,55 +3021,215 @@
       <c r="H38" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I38" s="35" t="s">
+      <c r="I38" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="J38" s="33"/>
-      <c r="K38" s="21" t="s">
+      <c r="J38" s="31"/>
+      <c r="K38" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="L38" s="21" t="s">
+      <c r="L38" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="76.8" customHeight="1" thickBot="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="15">
+    <row r="39" spans="1:26" ht="76.8" customHeight="1">
+      <c r="A39" s="68"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="67">
         <v>2</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="H39" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+    </row>
+    <row r="40" spans="1:26" ht="69.599999999999994" customHeight="1">
+      <c r="A40" s="69" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" s="70">
+        <v>44789</v>
+      </c>
+      <c r="C40" s="71" t="s">
+        <v>230</v>
+      </c>
+      <c r="D40" s="71" t="s">
+        <v>233</v>
+      </c>
+      <c r="E40" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" s="71">
+        <v>1</v>
+      </c>
+      <c r="H40" s="71" t="s">
+        <v>236</v>
+      </c>
+      <c r="I40" s="71" t="s">
+        <v>239</v>
+      </c>
+      <c r="J40" s="71"/>
+      <c r="K40" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="L40" s="72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="40.799999999999997" customHeight="1">
+      <c r="A41" s="73"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="72"/>
+      <c r="L41" s="72"/>
+    </row>
+    <row r="42" spans="1:26" ht="66.599999999999994" customHeight="1">
+      <c r="A42" s="75" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" s="76">
+        <v>44789</v>
+      </c>
+      <c r="C42" s="71" t="s">
+        <v>231</v>
+      </c>
+      <c r="D42" s="71" t="s">
+        <v>234</v>
+      </c>
+      <c r="E42" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="75">
+        <v>1</v>
+      </c>
+      <c r="H42" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="I42" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="J42" s="75"/>
+      <c r="K42" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="L42" s="71" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" ht="76.8" customHeight="1">
+      <c r="A43" s="71" t="s">
+        <v>241</v>
+      </c>
+      <c r="B43" s="70">
+        <v>44789</v>
+      </c>
+      <c r="C43" s="71" t="s">
+        <v>232</v>
+      </c>
+      <c r="D43" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="71">
+        <v>1</v>
+      </c>
+      <c r="H43" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="I43" s="71" t="s">
+        <v>239</v>
+      </c>
+      <c r="J43" s="71"/>
+      <c r="K43" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="L43" s="71" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="91">
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
+  <mergeCells count="94">
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="I22:I23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
@@ -2996,66 +3246,31 @@
     <mergeCell ref="I28:I29"/>
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="K28:K29"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
     <mergeCell ref="L32:L33"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H35" r:id="rId1" display="http://email.com/"/>
+    <hyperlink ref="H35" r:id="rId1" display="http://email.com/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3063,14 +3278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -3167,13 +3382,13 @@
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="25" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3181,13 +3396,13 @@
       <c r="B7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="25" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3195,13 +3410,13 @@
       <c r="B8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="25" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3209,13 +3424,13 @@
       <c r="B9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="25" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3223,13 +3438,13 @@
       <c r="B10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="25" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3237,10 +3452,10 @@
       <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="25" t="s">
         <v>192</v>
       </c>
       <c r="F11" t="s">
@@ -3251,10 +3466,10 @@
       <c r="B12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="25" t="s">
         <v>192</v>
       </c>
       <c r="F12" t="s">
@@ -3290,17 +3505,37 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1">
+    <row r="17" spans="1:6" ht="13.2">
+      <c r="A17" s="65"/>
       <c r="B17" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B18" s="2" t="s">
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+    </row>
+    <row r="18" spans="1:6" ht="66">
+      <c r="A18" s="65">
+        <v>44779</v>
+      </c>
+      <c r="B18" s="66" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" ht="15.75" customHeight="1">
+      <c r="C18" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="E18" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="F18" s="66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="B19" s="2" t="s">
         <v>96</v>
       </c>
@@ -3311,7 +3546,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15.75" customHeight="1">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="B20" s="2" t="s">
         <v>99</v>
       </c>
@@ -3322,7 +3557,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="B21" s="2" t="s">
         <v>104</v>
       </c>
@@ -3333,7 +3568,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="B22" s="2" t="s">
         <v>109</v>
       </c>
@@ -3344,7 +3579,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="B23" s="2" t="s">
         <v>110</v>
       </c>
@@ -3355,7 +3590,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="B24" s="2" t="s">
         <v>112</v>
       </c>
@@ -3363,7 +3598,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="B25" s="2" t="s">
         <v>119</v>
       </c>
@@ -3377,19 +3612,19 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="15.75" customHeight="1">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="B26" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C26" s="62" t="s">
+      <c r="C26" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="D26" s="62" t="s">
+      <c r="D26" s="25" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="63" t="s">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B27" s="26" t="s">
         <v>211</v>
       </c>
       <c r="C27" t="s">
@@ -3397,6 +3632,66 @@
       </c>
       <c r="D27" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="66">
+      <c r="A28" s="65">
+        <v>44779</v>
+      </c>
+      <c r="B28" s="66" t="s">
+        <v>228</v>
+      </c>
+      <c r="C28" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="D28" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="E28" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="F28" s="66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="66">
+      <c r="A29" s="65">
+        <v>44779</v>
+      </c>
+      <c r="B29" s="66" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="D29" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="E29" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="F29" s="66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="66">
+      <c r="A30" s="65">
+        <v>44779</v>
+      </c>
+      <c r="B30" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="C30" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="D30" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="E30" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="F30" s="66" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3406,7 +3701,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3421,7 +3716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3434,751 +3729,655 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="64" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="64" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="40" t="s">
+      <c r="H1" s="61"/>
+      <c r="I1" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="59" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="57">
         <v>44784</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G3" s="49">
+      <c r="G3" s="19">
         <v>1</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51" t="s">
+      <c r="I3" s="55"/>
+      <c r="J3" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="M3" s="51" t="s">
+      <c r="M3" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="47" t="s">
+      <c r="N3" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="51"/>
+      <c r="O3" s="50"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="49">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="19">
         <v>2</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="49">
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="19">
         <v>3</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="49">
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="19">
         <v>4</v>
       </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="42"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="49">
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="19">
         <v>5</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="44"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="42"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="42"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="44"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="52"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="44"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
+      <c r="A18" s="51"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="52"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="52"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="42"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="44"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="52"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="52"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="42"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="48"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="44"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="47"/>
+      <c r="A27" s="51"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="52"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="52"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="52"/>
-      <c r="O29" s="52"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="42"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="44"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
+      <c r="A31" s="51"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="52"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
-      <c r="O32" s="52"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="52"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="47"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="42"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="48"/>
+      <c r="O34" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="118">
-    <mergeCell ref="N31:N34"/>
-    <mergeCell ref="O31:O34"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="I31:I34"/>
-    <mergeCell ref="J31:J34"/>
-    <mergeCell ref="K31:K34"/>
-    <mergeCell ref="L31:L34"/>
-    <mergeCell ref="M31:M34"/>
-    <mergeCell ref="K27:K30"/>
-    <mergeCell ref="L27:L30"/>
-    <mergeCell ref="M27:M30"/>
-    <mergeCell ref="N27:N30"/>
-    <mergeCell ref="O27:O30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="N22:N26"/>
-    <mergeCell ref="O22:O26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="L22:L26"/>
-    <mergeCell ref="M22:M26"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="L18:L21"/>
-    <mergeCell ref="M18:M21"/>
-    <mergeCell ref="N18:N21"/>
-    <mergeCell ref="O18:O21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="O15:O17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="O8:O11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="M8:M11"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="A3:A7"/>
@@ -4201,9 +4400,105 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="O8:O11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="M8:M11"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="M18:M21"/>
+    <mergeCell ref="N18:N21"/>
+    <mergeCell ref="O18:O21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="N22:N26"/>
+    <mergeCell ref="O22:O26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="K22:K26"/>
+    <mergeCell ref="L22:L26"/>
+    <mergeCell ref="M22:M26"/>
+    <mergeCell ref="N31:N34"/>
+    <mergeCell ref="O31:O34"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="K31:K34"/>
+    <mergeCell ref="L31:L34"/>
+    <mergeCell ref="M31:M34"/>
+    <mergeCell ref="K27:K30"/>
+    <mergeCell ref="L27:L30"/>
+    <mergeCell ref="M27:M30"/>
+    <mergeCell ref="N27:N30"/>
+    <mergeCell ref="O27:O30"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="J3 J8 J12 J15 J18 J22 J27 J31">
+    <dataValidation type="list" allowBlank="1" sqref="J3 J8 J12 J15 J18 J22 J27 J31" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Reportado,En revisión,Finalizado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4213,7 +4508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
@@ -4228,228 +4523,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="24" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="60" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="23" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="59"/>
-      <c r="B7" s="60" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="60" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="59"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="59"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="59"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="59"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="59"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizacion Back end Casos de prueba
</commit_message>
<xml_diff>
--- a/Testing/Testing PI local.xlsx
+++ b/Testing/Testing PI local.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1p3p\OneDrive\Documentos\PI\grupo-09\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA118F-1A69-4C53-8DD8-7FBE44CA74BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BC7DD6-BB90-40AA-8F4E-5F2F9E00A49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Prueba" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="318">
   <si>
     <t>ID</t>
   </si>
@@ -787,6 +787,219 @@
   </si>
   <si>
     <t>visualizar categorias en la base de datos creadas por back</t>
+  </si>
+  <si>
+    <t>CP-030</t>
+  </si>
+  <si>
+    <t>Llamar categoria por id en postan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 categorias, por su id </t>
+  </si>
+  <si>
+    <t>CP-031</t>
+  </si>
+  <si>
+    <t>Validar put en postman</t>
+  </si>
+  <si>
+    <t>modificar categoria por id en postan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 categorias modificada, por su id </t>
+  </si>
+  <si>
+    <t>CP-032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear un producto </t>
+  </si>
+  <si>
+    <t>Generar la creacion de un producto en la base de datos</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Generar la peticion post para la ceacion de un nuevo item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un nuevo producto con id autoincremental </t>
+  </si>
+  <si>
+    <t>CP-033</t>
+  </si>
+  <si>
+    <t>Listar productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar la peticion para renderizar la lista de todos los productos disponibles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar peticion Get </t>
+  </si>
+  <si>
+    <t>Listado de todos los productos</t>
+  </si>
+  <si>
+    <t>CP-034</t>
+  </si>
+  <si>
+    <t>Listar por id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar el producto conociendo que id tiene </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con gett mas el id, listar el producto </t>
+  </si>
+  <si>
+    <t>Producto llamado por id</t>
+  </si>
+  <si>
+    <t>CP-035</t>
+  </si>
+  <si>
+    <t>Listar Ciudades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar la peticion para renderizar la lista de todos las ciudades disponibles </t>
+  </si>
+  <si>
+    <t>Listado de todas las ciudades</t>
+  </si>
+  <si>
+    <t>CP-036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear una ciudad </t>
+  </si>
+  <si>
+    <t>Generar la creacion de una ciudad en la base de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una nueva ciudad con id autoincremental </t>
+  </si>
+  <si>
+    <t>CP-037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar la ciudad conociendo que id tiene </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con get mas el id, listar la ciudad </t>
+  </si>
+  <si>
+    <t>una ciudad llamada por id</t>
+  </si>
+  <si>
+    <t>CP-038</t>
+  </si>
+  <si>
+    <t>Crear un feature</t>
+  </si>
+  <si>
+    <t>Generar la creacion de feature en la base de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un nuevo feature con id autoincremental </t>
+  </si>
+  <si>
+    <t>CP-039</t>
+  </si>
+  <si>
+    <t>Listar features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar la peticion para renderizar la lista de todos los features disponibles </t>
+  </si>
+  <si>
+    <t>Listado de todos los features</t>
+  </si>
+  <si>
+    <t>CP-040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar el feature conociendo que id tiene </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con get mas el id, listar el feature </t>
+  </si>
+  <si>
+    <t>Feature llamado por id</t>
+  </si>
+  <si>
+    <t>CP-041</t>
+  </si>
+  <si>
+    <t>Crear una  imagen</t>
+  </si>
+  <si>
+    <t>Generar la creacion de una imagen en la base de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una nueva imagen con id autoincremental </t>
+  </si>
+  <si>
+    <t>CP-042</t>
+  </si>
+  <si>
+    <t>Listar imágenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar la peticion para renderizar la lista de todos las imágenes disponibles </t>
+  </si>
+  <si>
+    <t>Listado de todos las imagenes</t>
+  </si>
+  <si>
+    <t>CP-043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar una imagen conociendo que id tiene </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con get mas el id, listar la imagen </t>
+  </si>
+  <si>
+    <t>Imagen llamada por id</t>
+  </si>
+  <si>
+    <t>CP-044</t>
+  </si>
+  <si>
+    <t>Crear una  politica</t>
+  </si>
+  <si>
+    <t>Generar la creacion de una politica en la base de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una nueva politica con id autoincremental </t>
+  </si>
+  <si>
+    <t>CP-045</t>
+  </si>
+  <si>
+    <t>Listar politicas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar la peticion para renderizar la lista de todos las politicas disponibles </t>
+  </si>
+  <si>
+    <t>Listado de todos las politicas</t>
+  </si>
+  <si>
+    <t>CP-046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar una politica conociendo que id tiene </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con get mas el id, listar la politica </t>
+  </si>
+  <si>
+    <t>Politica llamada por id</t>
   </si>
 </sst>
 </file>
@@ -811,11 +1024,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -823,6 +1038,7 @@
       <sz val="10"/>
       <color rgb="FF1F6166"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -836,6 +1052,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -848,10 +1065,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -943,7 +1162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1155,12 +1374,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF073763"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF073763"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF073763"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1227,31 +1459,62 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1263,46 +1526,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1314,38 +1570,24 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1567,11 +1809,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1585,46 +1827,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="37" t="s">
+      <c r="H1" s="51"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="48" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="13.8">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1634,11 +1876,11 @@
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-    </row>
-    <row r="3" spans="1:13" ht="79.2">
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+    </row>
+    <row r="3" spans="1:13" ht="66">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +1917,7 @@
       </c>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" ht="79.2">
+    <row r="4" spans="1:13" ht="66">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1926,7 +2168,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="105.6">
+    <row r="11" spans="1:13" ht="92.4">
       <c r="A11" s="26" t="s">
         <v>61</v>
       </c>
@@ -1963,7 +2205,7 @@
       </c>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="105.6">
+    <row r="12" spans="1:13" ht="92.4">
       <c r="A12" s="26" t="s">
         <v>65</v>
       </c>
@@ -2000,7 +2242,7 @@
       </c>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="105.6">
+    <row r="13" spans="1:13" ht="92.4">
       <c r="A13" s="26" t="s">
         <v>69</v>
       </c>
@@ -2037,7 +2279,7 @@
       </c>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:13" ht="158.4">
+    <row r="14" spans="1:13" ht="145.19999999999999">
       <c r="A14" s="26" t="s">
         <v>76</v>
       </c>
@@ -2229,16 +2471,16 @@
       <c r="B19" s="10">
         <v>44779</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="44" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="9">
@@ -2275,10 +2517,10 @@
     <row r="20" spans="1:26" ht="13.8" thickBot="1">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
       <c r="G20" s="9"/>
       <c r="H20" s="11"/>
       <c r="I20" s="9"/>
@@ -2300,13 +2542,13 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
     </row>
-    <row r="21" spans="1:26" ht="66.599999999999994" thickBot="1">
+    <row r="21" spans="1:26" ht="53.4" thickBot="1">
       <c r="A21" s="12"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="9">
         <v>2</v>
       </c>
@@ -2345,16 +2587,16 @@
       <c r="B22" s="10">
         <v>44779</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="44" t="s">
         <v>138</v>
       </c>
       <c r="G22" s="9">
@@ -2363,7 +2605,7 @@
       <c r="H22" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="44" t="s">
         <v>140</v>
       </c>
       <c r="J22" s="12"/>
@@ -2387,17 +2629,17 @@
     <row r="23" spans="1:26" ht="40.200000000000003" thickBot="1">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="9">
         <v>2</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I23" s="29"/>
+      <c r="I23" s="45"/>
       <c r="J23" s="12"/>
       <c r="K23" s="9" t="s">
         <v>93</v>
@@ -2427,16 +2669,16 @@
       <c r="B24" s="10">
         <v>44779</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="40" t="s">
         <v>144</v>
       </c>
       <c r="G24" s="11">
@@ -2445,7 +2687,7 @@
       <c r="H24" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="40" t="s">
         <v>98</v>
       </c>
       <c r="J24" s="12"/>
@@ -2473,17 +2715,17 @@
     <row r="25" spans="1:26" ht="40.200000000000003" thickBot="1">
       <c r="A25" s="12"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
       <c r="G25" s="11">
         <v>2</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="I25" s="35"/>
+      <c r="I25" s="41"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -2503,22 +2745,22 @@
       <c r="Z25" s="12"/>
     </row>
     <row r="26" spans="1:26" ht="40.200000000000003" thickBot="1">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="44">
+      <c r="B26" s="46">
         <v>44779</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="44" t="s">
         <v>95</v>
       </c>
       <c r="G26" s="9">
@@ -2527,7 +2769,7 @@
       <c r="H26" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="I26" s="28" t="s">
+      <c r="I26" s="44" t="s">
         <v>148</v>
       </c>
       <c r="J26" s="12"/>
@@ -2553,19 +2795,19 @@
       <c r="Z26" s="13"/>
     </row>
     <row r="27" spans="1:26" ht="53.4" thickBot="1">
-      <c r="A27" s="29"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="9">
         <v>2</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="I27" s="29"/>
+      <c r="I27" s="45"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="9" t="s">
@@ -2587,22 +2829,22 @@
       <c r="Z27" s="13"/>
     </row>
     <row r="28" spans="1:26" ht="39.6" customHeight="1" thickBot="1">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="40" t="s">
         <v>109</v>
       </c>
       <c r="B28" s="42">
         <v>44779</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="34" t="s">
+      <c r="F28" s="40" t="s">
         <v>105</v>
       </c>
       <c r="G28" s="11" t="s">
@@ -2611,14 +2853,14 @@
       <c r="H28" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="J28" s="34"/>
-      <c r="K28" s="28" t="s">
+      <c r="J28" s="40"/>
+      <c r="K28" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="28" t="s">
+      <c r="L28" s="44" t="s">
         <v>153</v>
       </c>
       <c r="M28" s="13"/>
@@ -2637,22 +2879,22 @@
       <c r="Z28" s="13"/>
     </row>
     <row r="29" spans="1:26" ht="40.200000000000003" thickBot="1">
-      <c r="A29" s="35"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="43"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="11" t="s">
         <v>154</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
@@ -2669,22 +2911,22 @@
       <c r="Z29" s="13"/>
     </row>
     <row r="30" spans="1:26" ht="72" customHeight="1" thickBot="1">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="44">
+      <c r="B30" s="46">
         <v>44779</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="44" t="s">
         <v>157</v>
       </c>
       <c r="G30" s="9">
@@ -2693,14 +2935,14 @@
       <c r="H30" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="I30" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28" t="s">
+      <c r="J30" s="44"/>
+      <c r="K30" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="L30" s="28" t="s">
+      <c r="L30" s="44" t="s">
         <v>133</v>
       </c>
       <c r="M30" s="13"/>
@@ -2719,22 +2961,22 @@
       <c r="Z30" s="13"/>
     </row>
     <row r="31" spans="1:26" ht="72.75" customHeight="1" thickBot="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="9">
         <v>2</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
@@ -2751,22 +2993,22 @@
       <c r="Z31" s="13"/>
     </row>
     <row r="32" spans="1:26" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="44">
+      <c r="B32" s="46">
         <v>44779</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="28" t="s">
+      <c r="F32" s="44" t="s">
         <v>111</v>
       </c>
       <c r="G32" s="9" t="s">
@@ -2775,14 +3017,14 @@
       <c r="H32" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="I32" s="28" t="s">
+      <c r="I32" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28" t="s">
+      <c r="J32" s="44"/>
+      <c r="K32" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="L32" s="28" t="s">
+      <c r="L32" s="44" t="s">
         <v>133</v>
       </c>
       <c r="M32" s="13"/>
@@ -2801,22 +3043,22 @@
       <c r="Z32" s="13"/>
     </row>
     <row r="33" spans="1:26" ht="79.8" thickBot="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
       <c r="G33" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
@@ -2833,22 +3075,22 @@
       <c r="Z33" s="13"/>
     </row>
     <row r="34" spans="1:26" ht="26.4" customHeight="1" thickBot="1">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="40" t="s">
         <v>119</v>
       </c>
       <c r="B34" s="42">
         <v>44779</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="40" t="s">
         <v>115</v>
       </c>
       <c r="G34" s="11">
@@ -2857,14 +3099,14 @@
       <c r="H34" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="I34" s="34" t="s">
+      <c r="I34" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="J34" s="34"/>
-      <c r="K34" s="28" t="s">
+      <c r="J34" s="40"/>
+      <c r="K34" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="L34" s="28" t="s">
+      <c r="L34" s="44" t="s">
         <v>153</v>
       </c>
       <c r="M34" s="13"/>
@@ -2883,22 +3125,22 @@
       <c r="Z34" s="13"/>
     </row>
     <row r="35" spans="1:26" ht="66.599999999999994" thickBot="1">
-      <c r="A35" s="35"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="43"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <v>2</v>
       </c>
       <c r="H35" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
@@ -2915,22 +3157,22 @@
       <c r="Z35" s="13"/>
     </row>
     <row r="36" spans="1:26" ht="66" customHeight="1" thickBot="1">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="40" t="s">
         <v>172</v>
       </c>
       <c r="B36" s="42">
         <v>44779</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="40" t="s">
         <v>168</v>
       </c>
       <c r="G36" s="11">
@@ -2939,14 +3181,14 @@
       <c r="H36" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="I36" s="34" t="s">
+      <c r="I36" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="J36" s="34"/>
-      <c r="K36" s="28" t="s">
+      <c r="J36" s="40"/>
+      <c r="K36" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="L36" s="28" t="s">
+      <c r="L36" s="44" t="s">
         <v>133</v>
       </c>
       <c r="M36" s="13"/>
@@ -2965,22 +3207,22 @@
       <c r="Z36" s="13"/>
     </row>
     <row r="37" spans="1:26" ht="53.4" thickBot="1">
-      <c r="A37" s="35"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="43"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <v>2</v>
       </c>
       <c r="H37" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
       <c r="O37" s="13"/>
@@ -2997,22 +3239,22 @@
       <c r="Z37" s="13"/>
     </row>
     <row r="38" spans="1:26" ht="53.4" customHeight="1">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="B38" s="32">
+      <c r="B38" s="57">
         <v>44779</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="30" t="s">
+      <c r="F38" s="54" t="s">
         <v>161</v>
       </c>
       <c r="G38" s="15">
@@ -3021,215 +3263,801 @@
       <c r="H38" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I38" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="J38" s="31"/>
-      <c r="K38" s="28" t="s">
+      <c r="J38" s="56"/>
+      <c r="K38" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="L38" s="28" t="s">
+      <c r="L38" s="44" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="76.8" customHeight="1">
-      <c r="A39" s="68"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="67">
+      <c r="A39" s="55"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="30">
         <v>2</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
     </row>
     <row r="40" spans="1:26" ht="69.599999999999994" customHeight="1">
-      <c r="A40" s="69" t="s">
+      <c r="A40" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="B40" s="70">
+      <c r="B40" s="31">
         <v>44789</v>
       </c>
-      <c r="C40" s="71" t="s">
+      <c r="C40" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="D40" s="71" t="s">
+      <c r="D40" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="E40" s="71" t="s">
+      <c r="E40" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="71" t="s">
+      <c r="F40" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="71">
+      <c r="G40" s="32">
         <v>1</v>
       </c>
-      <c r="H40" s="71" t="s">
+      <c r="H40" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="I40" s="71" t="s">
+      <c r="I40" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="J40" s="71"/>
-      <c r="K40" s="72" t="s">
+      <c r="J40" s="32"/>
+      <c r="K40" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="L40" s="72" t="s">
+      <c r="L40" s="39" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="40.799999999999997" customHeight="1">
-      <c r="A41" s="73"/>
-      <c r="B41" s="74"/>
-      <c r="C41" s="74"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="72"/>
-      <c r="L41" s="72"/>
+      <c r="A41" s="38"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
     </row>
     <row r="42" spans="1:26" ht="66.599999999999994" customHeight="1">
-      <c r="A42" s="75" t="s">
+      <c r="A42" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="B42" s="76">
+      <c r="B42" s="36">
         <v>44789</v>
       </c>
-      <c r="C42" s="71" t="s">
+      <c r="C42" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="D42" s="71" t="s">
+      <c r="D42" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="E42" s="75" t="s">
+      <c r="E42" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="71" t="s">
+      <c r="F42" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G42" s="75">
+      <c r="G42" s="35">
         <v>1</v>
       </c>
-      <c r="H42" s="71" t="s">
+      <c r="H42" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="I42" s="75" t="s">
+      <c r="I42" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="J42" s="75"/>
-      <c r="K42" s="75" t="s">
+      <c r="J42" s="35"/>
+      <c r="K42" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="L42" s="71" t="s">
+      <c r="L42" s="32" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="76.8" customHeight="1">
-      <c r="A43" s="71" t="s">
+    <row r="43" spans="1:26" ht="76.8" customHeight="1" thickBot="1">
+      <c r="A43" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="B43" s="70">
+      <c r="B43" s="31">
         <v>44789</v>
       </c>
-      <c r="C43" s="71" t="s">
+      <c r="C43" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="D43" s="71" t="s">
+      <c r="D43" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="E43" s="71" t="s">
+      <c r="E43" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="71" t="s">
+      <c r="F43" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G43" s="71">
+      <c r="G43" s="32">
         <v>1</v>
       </c>
-      <c r="H43" s="71" t="s">
+      <c r="H43" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="I43" s="71" t="s">
+      <c r="I43" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="J43" s="71"/>
-      <c r="K43" s="71" t="s">
+      <c r="J43" s="32"/>
+      <c r="K43" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="L43" s="71" t="s">
+      <c r="L43" s="32" t="s">
         <v>133</v>
       </c>
     </row>
+    <row r="44" spans="1:26" s="78" customFormat="1" ht="66">
+      <c r="A44" s="54" t="s">
+        <v>247</v>
+      </c>
+      <c r="B44" s="28">
+        <v>44795</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G44" s="29">
+        <v>1</v>
+      </c>
+      <c r="H44" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="I44" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="J44" s="29"/>
+      <c r="K44" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="L44" s="44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" s="78" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A45" s="79"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="45"/>
+    </row>
+    <row r="46" spans="1:26" s="78" customFormat="1" ht="66">
+      <c r="A46" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="B46" s="28">
+        <v>44795</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="29">
+        <v>1</v>
+      </c>
+      <c r="H46" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="I46" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="L46" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" s="80" customFormat="1" ht="66">
+      <c r="A47" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="B47" s="31">
+        <v>44792</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G47" s="32">
+        <v>1</v>
+      </c>
+      <c r="H47" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L47" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" s="78" customFormat="1" ht="79.2">
+      <c r="A48" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="B48" s="31">
+        <v>44792</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="E48" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G48" s="32">
+        <v>1</v>
+      </c>
+      <c r="H48" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I48" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L48" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="78" customFormat="1" ht="39.6">
+      <c r="A49" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="B49" s="31">
+        <v>44793</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="E49" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G49" s="32">
+        <v>1</v>
+      </c>
+      <c r="H49" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="I49" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L49" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="78" customFormat="1" ht="79.2">
+      <c r="A50" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" s="31">
+        <v>44793</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G50" s="32">
+        <v>1</v>
+      </c>
+      <c r="H50" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I50" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L50" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="78" customFormat="1" ht="66">
+      <c r="A51" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B51" s="31">
+        <v>44793</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="E51" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G51" s="32">
+        <v>1</v>
+      </c>
+      <c r="H51" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="I51" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L51" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="78" customFormat="1" ht="39.6">
+      <c r="A52" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B52" s="31">
+        <v>44793</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="E52" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G52" s="32">
+        <v>1</v>
+      </c>
+      <c r="H52" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="I52" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L52" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" s="78" customFormat="1" ht="66">
+      <c r="A53" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B53" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="E53" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G53" s="32">
+        <v>1</v>
+      </c>
+      <c r="H53" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="I53" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="J53" s="32"/>
+      <c r="K53" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L53" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="78" customFormat="1" ht="79.2">
+      <c r="A54" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="B54" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G54" s="32">
+        <v>1</v>
+      </c>
+      <c r="H54" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I54" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="J54" s="32"/>
+      <c r="K54" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L54" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="78" customFormat="1" ht="39.6">
+      <c r="A55" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="B55" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G55" s="32">
+        <v>1</v>
+      </c>
+      <c r="H55" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="I55" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="J55" s="32"/>
+      <c r="K55" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L55" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" s="78" customFormat="1" ht="66">
+      <c r="A56" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="B56" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="E56" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G56" s="32">
+        <v>1</v>
+      </c>
+      <c r="H56" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="I56" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L56" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="78" customFormat="1" ht="79.2">
+      <c r="A57" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="B57" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G57" s="32">
+        <v>1</v>
+      </c>
+      <c r="H57" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L57" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="78" customFormat="1" ht="39.6">
+      <c r="A58" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="B58" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="E58" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G58" s="32">
+        <v>1</v>
+      </c>
+      <c r="H58" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L58" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="78" customFormat="1" ht="66">
+      <c r="A59" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="B59" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D59" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="E59" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G59" s="32">
+        <v>1</v>
+      </c>
+      <c r="H59" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="I59" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="J59" s="32"/>
+      <c r="K59" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L59" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="78" customFormat="1" ht="79.2">
+      <c r="A60" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="B60" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="D60" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="E60" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G60" s="32">
+        <v>1</v>
+      </c>
+      <c r="H60" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="I60" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="J60" s="32"/>
+      <c r="K60" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L60" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="78" customFormat="1" ht="39.6">
+      <c r="A61" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="B61" s="31">
+        <v>44795</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="D61" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="E61" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="F61" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="G61" s="32">
+        <v>1</v>
+      </c>
+      <c r="H61" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="I61" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="J61" s="32"/>
+      <c r="K61" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L61" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="94">
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F22:F23"/>
+  <mergeCells count="97">
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D38:D39"/>
     <mergeCell ref="I22:I23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
@@ -3246,28 +4074,62 @@
     <mergeCell ref="I28:I29"/>
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="K28:K29"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H35" r:id="rId1" display="http://email.com/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3284,8 +4146,8 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -3506,32 +4368,32 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.2">
-      <c r="A17" s="65"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
     </row>
     <row r="18" spans="1:6" ht="66">
-      <c r="A18" s="65">
+      <c r="A18" s="28">
         <v>44779</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="E18" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="F18" s="66" t="s">
+      <c r="F18" s="29" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3635,62 +4497,62 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="66">
-      <c r="A28" s="65">
+      <c r="A28" s="28">
         <v>44779</v>
       </c>
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="E28" s="66" t="s">
+      <c r="E28" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="F28" s="66" t="s">
+      <c r="F28" s="29" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="66">
-      <c r="A29" s="65">
+      <c r="A29" s="28">
         <v>44779</v>
       </c>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="E29" s="66" t="s">
+      <c r="E29" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="F29" s="66" t="s">
+      <c r="F29" s="29" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="66">
-      <c r="A30" s="65">
+      <c r="A30" s="28">
         <v>44779</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="E30" s="66" t="s">
+      <c r="E30" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="F30" s="66" t="s">
+      <c r="F30" s="29" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3729,28 +4591,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="70" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="61"/>
+      <c r="H1" s="69"/>
       <c r="I1" s="59" t="s">
         <v>184</v>
       </c>
@@ -3774,43 +4636,43 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="63"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
       <c r="G2" s="18" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="B3" s="57">
+      <c r="B3" s="63">
         <v>44784</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="64" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="65" t="s">
         <v>199</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="65" t="s">
         <v>198</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="65" t="s">
         <v>201</v>
       </c>
       <c r="G3" s="19">
@@ -3819,565 +4681,659 @@
       <c r="H3" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="50" t="s">
+      <c r="I3" s="66"/>
+      <c r="J3" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="67" t="s">
         <v>202</v>
       </c>
-      <c r="L3" s="50" t="s">
+      <c r="L3" s="67" t="s">
         <v>203</v>
       </c>
-      <c r="M3" s="50" t="s">
+      <c r="M3" s="67" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="N3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="50"/>
+      <c r="O3" s="67"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
       <c r="G4" s="19">
         <v>2</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="19">
         <v>3</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
       <c r="G6" s="19">
         <v>4</v>
       </c>
       <c r="H6" s="19"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="19">
         <v>5</v>
       </c>
       <c r="H7" s="19"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="51"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="A8" s="61"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="62"/>
+      <c r="O9" s="62"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="47"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="51"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="56"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="75"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="47"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="48"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="49"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="74"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="65"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="62"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="60"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="65"/>
+      <c r="O18" s="65"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="47"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="47"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+      <c r="N22" s="65"/>
+      <c r="O22" s="65"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="47"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="62"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="51"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="46"/>
+      <c r="I27" s="66"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="47"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="62"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="48"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="47"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20"/>
       <c r="H32" s="21"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="62"/>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="47"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="47"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="62"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="62"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="48"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="118">
+    <mergeCell ref="O27:O30"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="K31:K34"/>
+    <mergeCell ref="L31:L34"/>
+    <mergeCell ref="M31:M34"/>
+    <mergeCell ref="K27:K30"/>
+    <mergeCell ref="L27:L30"/>
+    <mergeCell ref="M27:M30"/>
+    <mergeCell ref="N27:N30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="N22:N26"/>
+    <mergeCell ref="O22:O26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="K22:K26"/>
+    <mergeCell ref="L22:L26"/>
+    <mergeCell ref="M22:M26"/>
+    <mergeCell ref="N31:N34"/>
+    <mergeCell ref="O31:O34"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="M18:M21"/>
+    <mergeCell ref="N18:N21"/>
+    <mergeCell ref="O18:O21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="O8:O11"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="M8:M11"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="A3:A7"/>
@@ -4402,100 +5358,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="L3:L7"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="O8:O11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="M8:M11"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="O15:O17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="L18:L21"/>
-    <mergeCell ref="M18:M21"/>
-    <mergeCell ref="N18:N21"/>
-    <mergeCell ref="O18:O21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="N22:N26"/>
-    <mergeCell ref="O22:O26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="L22:L26"/>
-    <mergeCell ref="M22:M26"/>
-    <mergeCell ref="N31:N34"/>
-    <mergeCell ref="O31:O34"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="I31:I34"/>
-    <mergeCell ref="J31:J34"/>
-    <mergeCell ref="K31:K34"/>
-    <mergeCell ref="L31:L34"/>
-    <mergeCell ref="M31:M34"/>
-    <mergeCell ref="K27:K30"/>
-    <mergeCell ref="L27:L30"/>
-    <mergeCell ref="M27:M30"/>
-    <mergeCell ref="N27:N30"/>
-    <mergeCell ref="O27:O30"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="J3 J8 J12 J15 J18 J22 J27 J31" xr:uid="{00000000-0002-0000-0300-000000000000}">

</xml_diff>

<commit_message>
Casos de prueba sprint 2
</commit_message>
<xml_diff>
--- a/Testing/Testing PI local.xlsx
+++ b/Testing/Testing PI local.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1p3p\OneDrive\Documentos\PI\grupo-09\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dina\Documents\Desde aquí\grupo-09\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA118F-1A69-4C53-8DD8-7FBE44CA74BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-111" yWindow="-111" windowWidth="23254" windowHeight="12454"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Prueba" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="360">
   <si>
     <t>ID</t>
   </si>
@@ -788,11 +787,413 @@
   <si>
     <t>visualizar categorias en la base de datos creadas por back</t>
   </si>
+  <si>
+    <t>CDP-30</t>
+  </si>
+  <si>
+    <t>Validar ruta del home</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder contar con una ruta que me redireccione al home</t>
+  </si>
+  <si>
+    <t>Ingresar al aplicativo</t>
+  </si>
+  <si>
+    <t>Rutas amigables</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero contar con rutas amigables para facilitar mi busqueda</t>
+  </si>
+  <si>
+    <t>visualizar el detalle de los producto</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder visualizar el detalle de un producto</t>
+  </si>
+  <si>
+    <t>Estar registrado en la aplicación</t>
+  </si>
+  <si>
+    <t>llamado a la API</t>
+  </si>
+  <si>
+    <t>Yo como servicio quiero poder hacer un llamado a la API y que me retorne un producto</t>
+  </si>
+  <si>
+    <t>Visualizar detalle de un producto</t>
+  </si>
+  <si>
+    <t>Yo como cliente quiero poder visualizar el detalle de un producto responsive dentro del template implementado en el sprint 1</t>
+  </si>
+  <si>
+    <t>Probar flecha volver atras</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder visualizar la flecha volver atras y que esta me redireccione al home</t>
+  </si>
+  <si>
+    <t>validar 100% de la pantalla con los datos de ubicación</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero validar que el bloque con los datos de ubicación ocupe el 100% de la pantalla</t>
+  </si>
+  <si>
+    <t>-Estar logueado en la aplicación 
+-Estar en la vista Desktop
+-Haber seleccionado la Ciudad</t>
+  </si>
+  <si>
+    <t>Validar los datos de ubicación</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder visualizar un bloque con los datos de ubicación</t>
+  </si>
+  <si>
+    <t>Validar que la imagen principal ocupe la mitad de la pantalla y las demás imagenes ocupen la otra mitad en la vista Desktop</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero ver la imagen principal en la mitad del bloque y las otras imagenes en 2 columnas y 2 filas</t>
+  </si>
+  <si>
+    <t>Validar que los bordes sean redondeados sin ninguna acción</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero ver las imagenes con los bordes redondeados y que no realicen ninguna acción</t>
+  </si>
+  <si>
+    <t>-Estar logueado en la aplicación -Estar en la vista de Tablet y Phone -Haber seleccionado la Ciudad -Haber seleccionado el producto</t>
+  </si>
+  <si>
+    <t>Visualizar las grillas especificadas en la vista destokp</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero visualizar en la vista desktop una grilla de 4 columnas</t>
+  </si>
+  <si>
+    <t>Visualizar las grillas especificadas en la vista de Tablet</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero visualizar en la vista de tablet una grilla de 2 columnas</t>
+  </si>
+  <si>
+    <t>Visualizar las grillas especificadas en la vista de Phone</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero visualizar en la vista de phone una grilla de 1 columna</t>
+  </si>
+  <si>
+    <t>Visualizar las grillas especificadas de la politica de uso de un producto en la vista de Desktop</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder visualizar la politica de uso de un producto en una grilla de 3 columnas en la vista de desktop</t>
+  </si>
+  <si>
+    <t>Visualizar las grillas especificadas de la politica de uso de un producto en la vista de Tablet</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder visualizar la politica de uso de un producto en una grilla de 2 columnas en la vista de tablet</t>
+  </si>
+  <si>
+    <t>Visualizar las grillas especificadas de la politica de uso de un producto en la vista de Phone</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder visualizar la politica de uso de un producto en una grilla de 1 columna en la vista de phone</t>
+  </si>
+  <si>
+    <t>Validar las opciones de crear, listar y buscar por ID</t>
+  </si>
+  <si>
+    <t>Yo como administrador quiero poder crear, listar y buscar por id al controlador de productos</t>
+  </si>
+  <si>
+    <t>Validar el agregar categoría a un producto</t>
+  </si>
+  <si>
+    <t>Yo como administrador quiero agregar una categoria a un producto</t>
+  </si>
+  <si>
+    <t>Validar las caracteristicas de un producto</t>
+  </si>
+  <si>
+    <t>Yo como administrador quiero poder gestionar las caracteristicas de un producto</t>
+  </si>
+  <si>
+    <t>Validar el gestionar las ciudades para relacionarlas a un producto</t>
+  </si>
+  <si>
+    <t>Yo como administrador quiero poder gestionar las ciudades para relacionarlas a un producto</t>
+  </si>
+  <si>
+    <t>Validar ubicación de un producto por ciudad</t>
+  </si>
+  <si>
+    <t>Yo como administrador quiero poder indicar la ciudad de un producto para que el usuario pueda conocer su ubicación de manera mas sencilla</t>
+  </si>
+  <si>
+    <t>Gestionar las imagenes de un producto</t>
+  </si>
+  <si>
+    <t>Yo como administrador quiero poder gestionar las imagenes de un producto</t>
+  </si>
+  <si>
+    <t>Visualizar la lista de producto de en el home</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero visualizar la lista de productos en el home</t>
+  </si>
+  <si>
+    <t>Validar lista aleatoria en el home cuando no se esta logueado</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder ver la lista aleatoria en el home cuando no se esta logueado</t>
+  </si>
+  <si>
+    <t>Validar las busquedas por ciudad</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero realizar busquedas por ciudad</t>
+  </si>
+  <si>
+    <t>Validar el filtro por categorias</t>
+  </si>
+  <si>
+    <t>yo como usuario quiero poder filtrar por categorías para fecilitar mi busqueda</t>
+  </si>
+  <si>
+    <t>Validar calendario de fechas disponibles</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder visualizar las fechas disponibles para poder acceder a la sección de reservas</t>
+  </si>
+  <si>
+    <t>Validar acceso a cualquier hora y día de la semana</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero poder acceder 24/7 y de forma online al servicio de búsqueda de productos para poder consultar la información y reservar en cualquier momento.</t>
+  </si>
+  <si>
+    <t>1.Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido</t>
+  </si>
+  <si>
+    <t>1. Visualizar el botón ingresar
+2. Visualizar las opciones para colocar correo y contraseña
+3. El usuario debe poder ingresar a la aplicación</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido
+4. Seleccionar un producto</t>
+  </si>
+  <si>
+    <t>1. Visualizar el botón ingresar
+2. Visualizar las opciones para colocar correo y contraseña
+3. El usuario debe poder ingresar a la aplicación 
+4. Visualizar detalle del producto</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido
+4. Seleccionar un producto
+5.Dar click en la fecha volver atras</t>
+  </si>
+  <si>
+    <t>1. Visualizar el botón ingresar
+2. Visualizar las opciones para colocar correo y contraseña
+3. El usuario debe poder ingresar a la aplicación 
+4. Visualizar detalle del producto
+5. Debe redireccionar al home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido
+4. Seleccionar un producto
+</t>
+  </si>
+  <si>
+    <t>"1. Visualizar el botón ingresar
+2. Visualizar las opciones para colocar correo y contraseña
+3. El usuario debe poder ingresar a la aplicación 
+4. Visualizar detalle del producto al 100% de la pantalla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido
+4. Seleccionar una ciudad
+</t>
+  </si>
+  <si>
+    <t>1. Visualizar el botón ingresar
+2. Visualizar las opciones para colocar correo y contraseña
+3. El usuario debe poder ingresar a la aplicación 
+4. Visualizar los datos de la ubicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido
+4. Seleccionar una ciudad
+5.Seleccionar un producto
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Visualizar el botón ingresar
+2. Visualizar las opciones para colocar correo y contraseña
+3. El usuario debe poder ingresar a la aplicación 
+4. Visualizar los datos de la ubicación
+5. Visualizar detalle del producto al 100% de la pantalla
+</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido
+4. Seleccionar una ciudad 
+5.Seleccionar un producto</t>
+  </si>
+  <si>
+    <t>1. Visualizar el botón ingresar
+2. Visualizar las opciones para colocar correo y contraseña
+3. El usuario debe poder ingresar a la aplicación 
+4. Visualizar detalle del producto al 100% de la pantalla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar a la aplicación 
+2. Dar click al botón ingresar
+3. Colocar Email y contraseña valido
+4. Seleccionar una ciudad
+5. Seleccionar un producto
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Visualizar el botón ingresar
+2. Visualizar las opciones para colocar correo y contraseña
+3. El usuario debe poder ingresar a la aplicación 
+4. Visualizar los datos de ubicación
+5. Visualizar detalle del producto al 100% de la pantalla
+</t>
+  </si>
+  <si>
+    <t>ACEPTACIÓN</t>
+  </si>
+  <si>
+    <t>CDP-31</t>
+  </si>
+  <si>
+    <t>CDP-32</t>
+  </si>
+  <si>
+    <t>CDP-33</t>
+  </si>
+  <si>
+    <t>CDP-34</t>
+  </si>
+  <si>
+    <t>CDP-35</t>
+  </si>
+  <si>
+    <t>CDP-36</t>
+  </si>
+  <si>
+    <t>CDP-37</t>
+  </si>
+  <si>
+    <t>CDP-38</t>
+  </si>
+  <si>
+    <t>CDP-39</t>
+  </si>
+  <si>
+    <t>CDP-40</t>
+  </si>
+  <si>
+    <t>CDP-41</t>
+  </si>
+  <si>
+    <t>CDP-42</t>
+  </si>
+  <si>
+    <t>CDP-43</t>
+  </si>
+  <si>
+    <t>CDP-44</t>
+  </si>
+  <si>
+    <t>CDP-45</t>
+  </si>
+  <si>
+    <t>CDP-46</t>
+  </si>
+  <si>
+    <t>CDP-47</t>
+  </si>
+  <si>
+    <t>CDP-48</t>
+  </si>
+  <si>
+    <t>CDP-49</t>
+  </si>
+  <si>
+    <t>CDP-50</t>
+  </si>
+  <si>
+    <t>CDP-51</t>
+  </si>
+  <si>
+    <t>CDP-52</t>
+  </si>
+  <si>
+    <t>CDP-53</t>
+  </si>
+  <si>
+    <t>CDP-54</t>
+  </si>
+  <si>
+    <t>CDP-55</t>
+  </si>
+  <si>
+    <t>CDP-56</t>
+  </si>
+  <si>
+    <t>CDP-57</t>
+  </si>
+  <si>
+    <t>CDP-58</t>
+  </si>
+  <si>
+    <t>CDP-59</t>
+  </si>
+  <si>
+    <t>CDP-60</t>
+  </si>
+  <si>
+    <t>CDP-61</t>
+  </si>
+  <si>
+    <t>CDP-62</t>
+  </si>
+  <si>
+    <t>CDP-63</t>
+  </si>
+  <si>
+    <t>CDP-64</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -1160,7 +1561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1227,23 +1628,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1251,7 +1665,22 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1263,46 +1692,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1314,39 +1736,36 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1563,68 +1982,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Z78"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.69140625" customWidth="1"/>
+    <col min="3" max="3" width="12.53515625" customWidth="1"/>
+    <col min="4" max="4" width="29.53515625" customWidth="1"/>
+    <col min="5" max="5" width="12.53515625" customWidth="1"/>
+    <col min="7" max="7" width="6.07421875" customWidth="1"/>
+    <col min="8" max="8" width="18.84375" customWidth="1"/>
+    <col min="9" max="9" width="25.4609375" customWidth="1"/>
+    <col min="11" max="11" width="25.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.2">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:13" ht="12.9">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="37" t="s">
+      <c r="H1" s="50"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.8">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+    <row r="2" spans="1:13" ht="14.15">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1634,11 +2055,11 @@
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-    </row>
-    <row r="3" spans="1:13" ht="79.2">
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+    </row>
+    <row r="3" spans="1:13" ht="62.15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +2096,7 @@
       </c>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" ht="79.2">
+    <row r="4" spans="1:13" ht="62.15">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1712,7 +2133,7 @@
       </c>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:13" ht="79.2">
+    <row r="5" spans="1:13" ht="62.15">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1749,7 +2170,7 @@
       </c>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:13" ht="79.2">
+    <row r="6" spans="1:13" ht="49.75">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1786,7 +2207,7 @@
       </c>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:13" ht="79.2">
+    <row r="7" spans="1:13" ht="74.599999999999994">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -1823,7 +2244,7 @@
       </c>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="79.2">
+    <row r="8" spans="1:13" ht="74.599999999999994">
       <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
@@ -1860,7 +2281,7 @@
       </c>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13" ht="118.8">
+    <row r="9" spans="1:13" ht="74.599999999999994">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -1897,7 +2318,7 @@
       </c>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="1:13" ht="109.8" customHeight="1">
+    <row r="10" spans="1:13" ht="62.15">
       <c r="A10" s="26" t="s">
         <v>55</v>
       </c>
@@ -1926,7 +2347,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="105.6">
+    <row r="11" spans="1:13" ht="87">
       <c r="A11" s="26" t="s">
         <v>61</v>
       </c>
@@ -1963,7 +2384,7 @@
       </c>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="105.6">
+    <row r="12" spans="1:13" ht="87">
       <c r="A12" s="26" t="s">
         <v>65</v>
       </c>
@@ -2000,7 +2421,7 @@
       </c>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="105.6">
+    <row r="13" spans="1:13" ht="87">
       <c r="A13" s="26" t="s">
         <v>69</v>
       </c>
@@ -2037,7 +2458,7 @@
       </c>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:13" ht="158.4">
+    <row r="14" spans="1:13" ht="99.45">
       <c r="A14" s="26" t="s">
         <v>76</v>
       </c>
@@ -2074,7 +2495,7 @@
       </c>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:13" ht="132">
+    <row r="15" spans="1:13" ht="99.45">
       <c r="A15" s="26" t="s">
         <v>81</v>
       </c>
@@ -2111,7 +2532,7 @@
       </c>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:13" ht="92.4">
+    <row r="16" spans="1:13" ht="87">
       <c r="A16" s="26" t="s">
         <v>87</v>
       </c>
@@ -2148,7 +2569,7 @@
       </c>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:26" ht="92.4">
+    <row r="17" spans="1:26" ht="87">
       <c r="A17" s="26" t="s">
         <v>89</v>
       </c>
@@ -2185,7 +2606,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:26" ht="93" thickBot="1">
+    <row r="18" spans="1:26" ht="87.45" thickBot="1">
       <c r="A18" s="26" t="s">
         <v>91</v>
       </c>
@@ -2222,23 +2643,23 @@
       </c>
       <c r="M18" s="5"/>
     </row>
-    <row r="19" spans="1:26" ht="40.200000000000003" thickBot="1">
+    <row r="19" spans="1:26" ht="25.3" thickBot="1">
       <c r="A19" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B19" s="10">
         <v>44779</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="43" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="9">
@@ -2272,13 +2693,13 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="13.8" thickBot="1">
+    <row r="20" spans="1:26" ht="12.9" thickBot="1">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
       <c r="G20" s="9"/>
       <c r="H20" s="11"/>
       <c r="I20" s="9"/>
@@ -2300,13 +2721,13 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
     </row>
-    <row r="21" spans="1:26" ht="66.599999999999994" thickBot="1">
+    <row r="21" spans="1:26" ht="37.75" thickBot="1">
       <c r="A21" s="12"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
       <c r="G21" s="9">
         <v>2</v>
       </c>
@@ -2338,23 +2759,23 @@
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
     </row>
-    <row r="22" spans="1:26" ht="26.4" customHeight="1" thickBot="1">
+    <row r="22" spans="1:26" ht="12.9" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B22" s="10">
         <v>44779</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="43" t="s">
         <v>138</v>
       </c>
       <c r="G22" s="9">
@@ -2363,7 +2784,7 @@
       <c r="H22" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="43" t="s">
         <v>140</v>
       </c>
       <c r="J22" s="12"/>
@@ -2384,20 +2805,20 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
     </row>
-    <row r="23" spans="1:26" ht="40.200000000000003" thickBot="1">
+    <row r="23" spans="1:26" ht="37.75" thickBot="1">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
       <c r="G23" s="9">
         <v>2</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I23" s="29"/>
+      <c r="I23" s="44"/>
       <c r="J23" s="12"/>
       <c r="K23" s="9" t="s">
         <v>93</v>
@@ -2420,23 +2841,23 @@
       <c r="Y23" s="12"/>
       <c r="Z23" s="12"/>
     </row>
-    <row r="24" spans="1:26" ht="40.200000000000003" thickBot="1">
+    <row r="24" spans="1:26" ht="25.3" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B24" s="10">
         <v>44779</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="39" t="s">
         <v>144</v>
       </c>
       <c r="G24" s="11">
@@ -2445,7 +2866,7 @@
       <c r="H24" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="39" t="s">
         <v>98</v>
       </c>
       <c r="J24" s="12"/>
@@ -2470,20 +2891,20 @@
       <c r="Y24" s="12"/>
       <c r="Z24" s="12"/>
     </row>
-    <row r="25" spans="1:26" ht="40.200000000000003" thickBot="1">
+    <row r="25" spans="1:26" ht="25.3" thickBot="1">
       <c r="A25" s="12"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
       <c r="G25" s="11">
         <v>2</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="I25" s="35"/>
+      <c r="I25" s="40"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -2502,23 +2923,23 @@
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
     </row>
-    <row r="26" spans="1:26" ht="40.200000000000003" thickBot="1">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:26" ht="25.3" thickBot="1">
+      <c r="A26" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="44">
+      <c r="B26" s="45">
         <v>44779</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="43" t="s">
         <v>95</v>
       </c>
       <c r="G26" s="9">
@@ -2527,7 +2948,7 @@
       <c r="H26" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="I26" s="28" t="s">
+      <c r="I26" s="43" t="s">
         <v>148</v>
       </c>
       <c r="J26" s="12"/>
@@ -2552,20 +2973,20 @@
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
     </row>
-    <row r="27" spans="1:26" ht="53.4" thickBot="1">
-      <c r="A27" s="29"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+    <row r="27" spans="1:26" ht="25.3" thickBot="1">
+      <c r="A27" s="44"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
       <c r="G27" s="9">
         <v>2</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="I27" s="29"/>
+      <c r="I27" s="44"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="9" t="s">
@@ -2586,23 +3007,23 @@
       <c r="Y27" s="13"/>
       <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:26" ht="39.6" customHeight="1" thickBot="1">
-      <c r="A28" s="34" t="s">
+    <row r="28" spans="1:26" ht="37.75" thickBot="1">
+      <c r="A28" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="42">
+      <c r="B28" s="41">
         <v>44779</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="34" t="s">
+      <c r="F28" s="39" t="s">
         <v>105</v>
       </c>
       <c r="G28" s="11" t="s">
@@ -2611,14 +3032,14 @@
       <c r="H28" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="J28" s="34"/>
-      <c r="K28" s="28" t="s">
+      <c r="J28" s="39"/>
+      <c r="K28" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="28" t="s">
+      <c r="L28" s="43" t="s">
         <v>153</v>
       </c>
       <c r="M28" s="13"/>
@@ -2636,23 +3057,23 @@
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:26" ht="40.200000000000003" thickBot="1">
-      <c r="A29" s="35"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
+    <row r="29" spans="1:26" ht="25.3" thickBot="1">
+      <c r="A29" s="40"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
       <c r="G29" s="11" t="s">
         <v>154</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
@@ -2668,23 +3089,23 @@
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:26" ht="72" customHeight="1" thickBot="1">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:26" ht="12.9" thickBot="1">
+      <c r="A30" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="44">
+      <c r="B30" s="45">
         <v>44779</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="43" t="s">
         <v>157</v>
       </c>
       <c r="G30" s="9">
@@ -2693,14 +3114,14 @@
       <c r="H30" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="I30" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28" t="s">
+      <c r="J30" s="43"/>
+      <c r="K30" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="L30" s="28" t="s">
+      <c r="L30" s="43" t="s">
         <v>133</v>
       </c>
       <c r="M30" s="13"/>
@@ -2718,23 +3139,23 @@
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:26" ht="72.75" customHeight="1" thickBot="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
+    <row r="31" spans="1:26" ht="25.3" thickBot="1">
+      <c r="A31" s="44"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
       <c r="G31" s="9">
         <v>2</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
@@ -2750,23 +3171,23 @@
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
     </row>
-    <row r="32" spans="1:26" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A32" s="28" t="s">
+    <row r="32" spans="1:26" ht="12.9" thickBot="1">
+      <c r="A32" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="44">
+      <c r="B32" s="45">
         <v>44779</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="28" t="s">
+      <c r="F32" s="43" t="s">
         <v>111</v>
       </c>
       <c r="G32" s="9" t="s">
@@ -2775,14 +3196,14 @@
       <c r="H32" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="I32" s="28" t="s">
+      <c r="I32" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28" t="s">
+      <c r="J32" s="43"/>
+      <c r="K32" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="L32" s="28" t="s">
+      <c r="L32" s="43" t="s">
         <v>133</v>
       </c>
       <c r="M32" s="13"/>
@@ -2800,23 +3221,23 @@
       <c r="Y32" s="13"/>
       <c r="Z32" s="13"/>
     </row>
-    <row r="33" spans="1:26" ht="79.8" thickBot="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
+    <row r="33" spans="1:26" ht="50.15" thickBot="1">
+      <c r="A33" s="44"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
       <c r="G33" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
@@ -2832,23 +3253,23 @@
       <c r="Y33" s="13"/>
       <c r="Z33" s="13"/>
     </row>
-    <row r="34" spans="1:26" ht="26.4" customHeight="1" thickBot="1">
-      <c r="A34" s="34" t="s">
+    <row r="34" spans="1:26" ht="12.9" thickBot="1">
+      <c r="A34" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="42">
+      <c r="B34" s="41">
         <v>44779</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="39" t="s">
         <v>115</v>
       </c>
       <c r="G34" s="11">
@@ -2857,14 +3278,14 @@
       <c r="H34" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="I34" s="34" t="s">
+      <c r="I34" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="J34" s="34"/>
-      <c r="K34" s="28" t="s">
+      <c r="J34" s="39"/>
+      <c r="K34" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="L34" s="28" t="s">
+      <c r="L34" s="43" t="s">
         <v>153</v>
       </c>
       <c r="M34" s="13"/>
@@ -2882,23 +3303,23 @@
       <c r="Y34" s="13"/>
       <c r="Z34" s="13"/>
     </row>
-    <row r="35" spans="1:26" ht="66.599999999999994" thickBot="1">
-      <c r="A35" s="35"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
+    <row r="35" spans="1:26" ht="37.75" thickBot="1">
+      <c r="A35" s="40"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="11">
         <v>2</v>
       </c>
       <c r="H35" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
@@ -2914,23 +3335,23 @@
       <c r="Y35" s="13"/>
       <c r="Z35" s="13"/>
     </row>
-    <row r="36" spans="1:26" ht="66" customHeight="1" thickBot="1">
-      <c r="A36" s="34" t="s">
+    <row r="36" spans="1:26" ht="25.3" thickBot="1">
+      <c r="A36" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="B36" s="42">
+      <c r="B36" s="41">
         <v>44779</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="39" t="s">
         <v>168</v>
       </c>
       <c r="G36" s="11">
@@ -2939,14 +3360,14 @@
       <c r="H36" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="I36" s="34" t="s">
+      <c r="I36" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="J36" s="34"/>
-      <c r="K36" s="28" t="s">
+      <c r="J36" s="39"/>
+      <c r="K36" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="L36" s="28" t="s">
+      <c r="L36" s="43" t="s">
         <v>133</v>
       </c>
       <c r="M36" s="13"/>
@@ -2964,23 +3385,23 @@
       <c r="Y36" s="13"/>
       <c r="Z36" s="13"/>
     </row>
-    <row r="37" spans="1:26" ht="53.4" thickBot="1">
-      <c r="A37" s="35"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+    <row r="37" spans="1:26" ht="37.75" thickBot="1">
+      <c r="A37" s="40"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="11">
         <v>2</v>
       </c>
       <c r="H37" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
       <c r="O37" s="13"/>
@@ -2996,23 +3417,23 @@
       <c r="Y37" s="13"/>
       <c r="Z37" s="13"/>
     </row>
-    <row r="38" spans="1:26" ht="53.4" customHeight="1">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:26" ht="12.45">
+      <c r="A38" s="53" t="s">
         <v>211</v>
       </c>
-      <c r="B38" s="32">
+      <c r="B38" s="56">
         <v>44779</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="55" t="s">
         <v>173</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="30" t="s">
+      <c r="F38" s="53" t="s">
         <v>161</v>
       </c>
       <c r="G38" s="15">
@@ -3021,215 +3442,1306 @@
       <c r="H38" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I38" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="J38" s="31"/>
-      <c r="K38" s="28" t="s">
+      <c r="J38" s="55"/>
+      <c r="K38" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="L38" s="28" t="s">
+      <c r="L38" s="43" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="76.8" customHeight="1">
-      <c r="A39" s="68"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="67">
+    <row r="39" spans="1:26" ht="24.9">
+      <c r="A39" s="54"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="30">
         <v>2</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-    </row>
-    <row r="40" spans="1:26" ht="69.599999999999994" customHeight="1">
-      <c r="A40" s="69" t="s">
+      <c r="I39" s="54"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+    </row>
+    <row r="40" spans="1:26" ht="37.299999999999997">
+      <c r="A40" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B40" s="70">
+      <c r="B40" s="31">
         <v>44789</v>
       </c>
-      <c r="C40" s="71" t="s">
+      <c r="C40" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="D40" s="71" t="s">
+      <c r="D40" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="E40" s="71" t="s">
+      <c r="E40" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="71" t="s">
+      <c r="F40" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="71">
+      <c r="G40" s="32">
         <v>1</v>
       </c>
-      <c r="H40" s="71" t="s">
+      <c r="H40" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="I40" s="71" t="s">
+      <c r="I40" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="J40" s="71"/>
-      <c r="K40" s="72" t="s">
+      <c r="J40" s="32"/>
+      <c r="K40" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="L40" s="72" t="s">
+      <c r="L40" s="38" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="40.799999999999997" customHeight="1">
-      <c r="A41" s="73"/>
-      <c r="B41" s="74"/>
-      <c r="C41" s="74"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="72"/>
-      <c r="L41" s="72"/>
-    </row>
-    <row r="42" spans="1:26" ht="66.599999999999994" customHeight="1">
-      <c r="A42" s="75" t="s">
+    <row r="41" spans="1:26" ht="12.45">
+      <c r="A41" s="37"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+    </row>
+    <row r="42" spans="1:26" ht="37.299999999999997">
+      <c r="A42" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="B42" s="76">
+      <c r="B42" s="35">
         <v>44789</v>
       </c>
-      <c r="C42" s="71" t="s">
+      <c r="C42" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="D42" s="71" t="s">
+      <c r="D42" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="E42" s="75" t="s">
+      <c r="E42" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="71" t="s">
+      <c r="F42" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G42" s="75">
+      <c r="G42" s="34">
         <v>1</v>
       </c>
-      <c r="H42" s="71" t="s">
+      <c r="H42" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="I42" s="75" t="s">
+      <c r="I42" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="J42" s="75"/>
-      <c r="K42" s="75" t="s">
+      <c r="J42" s="34"/>
+      <c r="K42" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="L42" s="71" t="s">
+      <c r="L42" s="32" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="76.8" customHeight="1">
-      <c r="A43" s="71" t="s">
+    <row r="43" spans="1:26" ht="24.9">
+      <c r="A43" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="B43" s="70">
+      <c r="B43" s="31">
         <v>44789</v>
       </c>
-      <c r="C43" s="71" t="s">
+      <c r="C43" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="D43" s="71" t="s">
+      <c r="D43" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="E43" s="71" t="s">
+      <c r="E43" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="71" t="s">
+      <c r="F43" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G43" s="71">
+      <c r="G43" s="32">
         <v>1</v>
       </c>
-      <c r="H43" s="71" t="s">
+      <c r="H43" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="I43" s="71" t="s">
+      <c r="I43" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="J43" s="71"/>
-      <c r="K43" s="71" t="s">
+      <c r="J43" s="32"/>
+      <c r="K43" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="L43" s="71" t="s">
+      <c r="L43" s="32" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" ht="74.599999999999994">
+      <c r="A44" t="s">
+        <v>247</v>
+      </c>
+      <c r="B44" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C44" s="78" t="s">
+        <v>248</v>
+      </c>
+      <c r="D44" s="78" t="s">
+        <v>249</v>
+      </c>
+      <c r="E44" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="82" t="s">
+        <v>250</v>
+      </c>
+      <c r="H44" s="82" t="s">
+        <v>308</v>
+      </c>
+      <c r="I44" s="78" t="s">
+        <v>309</v>
+      </c>
+      <c r="J44" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K44" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L44" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" ht="74.599999999999994">
+      <c r="A45" t="s">
+        <v>326</v>
+      </c>
+      <c r="B45" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C45" s="78" t="s">
+        <v>251</v>
+      </c>
+      <c r="D45" s="78" t="s">
+        <v>252</v>
+      </c>
+      <c r="E45" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="82" t="s">
+        <v>250</v>
+      </c>
+      <c r="H45" s="78" t="s">
+        <v>310</v>
+      </c>
+      <c r="I45" s="78" t="s">
+        <v>309</v>
+      </c>
+      <c r="J45" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K45" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L45" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" ht="99.45">
+      <c r="A46" t="s">
+        <v>327</v>
+      </c>
+      <c r="B46" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C46" s="78" t="s">
+        <v>253</v>
+      </c>
+      <c r="D46" s="78" t="s">
+        <v>254</v>
+      </c>
+      <c r="E46" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="82" t="s">
+        <v>255</v>
+      </c>
+      <c r="H46" s="78" t="s">
+        <v>311</v>
+      </c>
+      <c r="I46" s="78" t="s">
+        <v>312</v>
+      </c>
+      <c r="J46" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K46" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L46" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" ht="37.299999999999997">
+      <c r="A47" t="s">
+        <v>328</v>
+      </c>
+      <c r="B47" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C47" s="78" t="s">
+        <v>256</v>
+      </c>
+      <c r="D47" s="78" t="s">
+        <v>257</v>
+      </c>
+      <c r="E47" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F47" s="82" t="s">
+        <v>255</v>
+      </c>
+      <c r="H47" s="78"/>
+      <c r="I47" s="78"/>
+      <c r="J47" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K47" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L47" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" ht="99.45">
+      <c r="A48" t="s">
+        <v>329</v>
+      </c>
+      <c r="B48" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C48" s="78" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="78" t="s">
+        <v>259</v>
+      </c>
+      <c r="E48" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="82" t="s">
+        <v>255</v>
+      </c>
+      <c r="H48" s="78" t="s">
+        <v>311</v>
+      </c>
+      <c r="I48" s="78" t="s">
+        <v>312</v>
+      </c>
+      <c r="J48" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K48" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L48" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="124.3">
+      <c r="A49" t="s">
+        <v>330</v>
+      </c>
+      <c r="B49" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C49" s="78" t="s">
+        <v>260</v>
+      </c>
+      <c r="D49" s="78" t="s">
+        <v>261</v>
+      </c>
+      <c r="E49" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="82" t="s">
+        <v>255</v>
+      </c>
+      <c r="H49" s="78" t="s">
+        <v>313</v>
+      </c>
+      <c r="I49" s="81" t="s">
+        <v>314</v>
+      </c>
+      <c r="J49" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K49" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L49" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="111.9">
+      <c r="A50" t="s">
+        <v>331</v>
+      </c>
+      <c r="B50" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C50" s="78" t="s">
+        <v>262</v>
+      </c>
+      <c r="D50" s="78" t="s">
+        <v>263</v>
+      </c>
+      <c r="E50" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H50" s="78" t="s">
+        <v>315</v>
+      </c>
+      <c r="I50" s="81" t="s">
+        <v>316</v>
+      </c>
+      <c r="J50" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K50" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L50" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="111.9">
+      <c r="A51" t="s">
+        <v>332</v>
+      </c>
+      <c r="B51" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C51" s="78" t="s">
+        <v>265</v>
+      </c>
+      <c r="D51" s="78" t="s">
+        <v>266</v>
+      </c>
+      <c r="E51" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H51" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="I51" s="81" t="s">
+        <v>318</v>
+      </c>
+      <c r="J51" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K51" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L51" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="136.75">
+      <c r="A52" t="s">
+        <v>333</v>
+      </c>
+      <c r="B52" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C52" s="78" t="s">
+        <v>267</v>
+      </c>
+      <c r="D52" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="E52" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H52" s="78" t="s">
+        <v>319</v>
+      </c>
+      <c r="I52" s="81" t="s">
+        <v>320</v>
+      </c>
+      <c r="J52" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K52" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L52" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="124.3">
+      <c r="A53" t="s">
+        <v>334</v>
+      </c>
+      <c r="B53" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C53" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="E53" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H53" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="I53" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="J53" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K53" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L53" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="124.3">
+      <c r="A54" t="s">
+        <v>335</v>
+      </c>
+      <c r="B54" s="77">
+        <v>44792</v>
+      </c>
+      <c r="C54" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="D54" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="E54" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H54" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="I54" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="J54" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K54" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L54" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="124.3">
+      <c r="A55" t="s">
+        <v>336</v>
+      </c>
+      <c r="B55" s="77">
+        <v>44793</v>
+      </c>
+      <c r="C55" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="D55" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="E55" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H55" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="I55" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="J55" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K55" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L55" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="124.3">
+      <c r="A56" t="s">
+        <v>337</v>
+      </c>
+      <c r="B56" s="77">
+        <v>44794</v>
+      </c>
+      <c r="C56" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="D56" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="E56" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H56" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="I56" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="J56" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K56" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L56" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="124.3">
+      <c r="A57" t="s">
+        <v>338</v>
+      </c>
+      <c r="B57" s="77">
+        <v>44795</v>
+      </c>
+      <c r="C57" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="D57" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="E57" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H57" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="I57" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="J57" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K57" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L57" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="124.3">
+      <c r="A58" t="s">
+        <v>339</v>
+      </c>
+      <c r="B58" s="77">
+        <v>44796</v>
+      </c>
+      <c r="C58" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="D58" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="E58" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H58" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="I58" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="J58" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K58" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L58" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="124.3">
+      <c r="A59" t="s">
+        <v>340</v>
+      </c>
+      <c r="B59" s="77">
+        <v>44797</v>
+      </c>
+      <c r="C59" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="D59" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="E59" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H59" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="I59" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="J59" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K59" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L59" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="124.3">
+      <c r="A60" t="s">
+        <v>341</v>
+      </c>
+      <c r="B60" s="77">
+        <v>44798</v>
+      </c>
+      <c r="C60" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="D60" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="E60" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="H60" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="I60" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="J60" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K60" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L60" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="149.15">
+      <c r="A61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B61" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C61" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="D61" s="78" t="s">
+        <v>273</v>
+      </c>
+      <c r="E61" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="82" t="s">
+        <v>271</v>
+      </c>
+      <c r="H61" s="78" t="s">
+        <v>323</v>
+      </c>
+      <c r="I61" s="81" t="s">
+        <v>324</v>
+      </c>
+      <c r="J61" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K61" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L61" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="149.15">
+      <c r="A62" t="s">
+        <v>343</v>
+      </c>
+      <c r="B62" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C62" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="D62" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="E62" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="82" t="s">
+        <v>271</v>
+      </c>
+      <c r="H62" s="78" t="s">
+        <v>323</v>
+      </c>
+      <c r="I62" s="81" t="s">
+        <v>324</v>
+      </c>
+      <c r="J62" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K62" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L62" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="149.15">
+      <c r="A63" t="s">
+        <v>344</v>
+      </c>
+      <c r="B63" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C63" s="79" t="s">
+        <v>276</v>
+      </c>
+      <c r="D63" s="78" t="s">
+        <v>277</v>
+      </c>
+      <c r="E63" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="82" t="s">
+        <v>271</v>
+      </c>
+      <c r="H63" s="78" t="s">
+        <v>323</v>
+      </c>
+      <c r="I63" s="81" t="s">
+        <v>324</v>
+      </c>
+      <c r="J63" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K63" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L63" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="149.15">
+      <c r="A64" t="s">
+        <v>345</v>
+      </c>
+      <c r="B64" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C64" s="79" t="s">
+        <v>278</v>
+      </c>
+      <c r="D64" s="78" t="s">
+        <v>279</v>
+      </c>
+      <c r="E64" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" s="82" t="s">
+        <v>271</v>
+      </c>
+      <c r="H64" s="78" t="s">
+        <v>323</v>
+      </c>
+      <c r="I64" s="81" t="s">
+        <v>324</v>
+      </c>
+      <c r="J64" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K64" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L64" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="149.15">
+      <c r="A65" t="s">
+        <v>346</v>
+      </c>
+      <c r="B65" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C65" s="79" t="s">
+        <v>280</v>
+      </c>
+      <c r="D65" s="78" t="s">
+        <v>281</v>
+      </c>
+      <c r="E65" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="82" t="s">
+        <v>271</v>
+      </c>
+      <c r="H65" s="78" t="s">
+        <v>323</v>
+      </c>
+      <c r="I65" s="81" t="s">
+        <v>324</v>
+      </c>
+      <c r="J65" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K65" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L65" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="149.15">
+      <c r="A66" t="s">
+        <v>347</v>
+      </c>
+      <c r="B66" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C66" s="79" t="s">
+        <v>282</v>
+      </c>
+      <c r="D66" s="78" t="s">
+        <v>283</v>
+      </c>
+      <c r="E66" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="82" t="s">
+        <v>271</v>
+      </c>
+      <c r="H66" s="78" t="s">
+        <v>323</v>
+      </c>
+      <c r="I66" s="81" t="s">
+        <v>324</v>
+      </c>
+      <c r="J66" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K66" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L66" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="49.75">
+      <c r="A67" t="s">
+        <v>348</v>
+      </c>
+      <c r="B67" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C67" s="78" t="s">
+        <v>284</v>
+      </c>
+      <c r="D67" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="E67" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F67" s="78"/>
+      <c r="J67" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K67" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L67" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="49.75">
+      <c r="A68" t="s">
+        <v>349</v>
+      </c>
+      <c r="B68" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C68" s="78" t="s">
+        <v>286</v>
+      </c>
+      <c r="D68" s="78" t="s">
+        <v>287</v>
+      </c>
+      <c r="E68" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F68" s="78"/>
+      <c r="J68" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K68" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L68" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="37.299999999999997">
+      <c r="A69" t="s">
+        <v>350</v>
+      </c>
+      <c r="B69" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C69" s="78" t="s">
+        <v>288</v>
+      </c>
+      <c r="D69" s="78" t="s">
+        <v>289</v>
+      </c>
+      <c r="E69" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F69" s="78"/>
+      <c r="J69" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K69" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L69" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="62.15">
+      <c r="A70" t="s">
+        <v>351</v>
+      </c>
+      <c r="B70" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C70" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="D70" s="78" t="s">
+        <v>291</v>
+      </c>
+      <c r="E70" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F70" s="78"/>
+      <c r="J70" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K70" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L70" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="49.75">
+      <c r="A71" t="s">
+        <v>352</v>
+      </c>
+      <c r="B71" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C71" s="78" t="s">
+        <v>292</v>
+      </c>
+      <c r="D71" s="78" t="s">
+        <v>293</v>
+      </c>
+      <c r="E71" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F71" s="78"/>
+      <c r="J71" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K71" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L71" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="37.299999999999997">
+      <c r="A72" t="s">
+        <v>353</v>
+      </c>
+      <c r="B72" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C72" s="78" t="s">
+        <v>294</v>
+      </c>
+      <c r="D72" s="78" t="s">
+        <v>295</v>
+      </c>
+      <c r="E72" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F72" s="78"/>
+      <c r="J72" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K72" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L72" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="49.75">
+      <c r="A73" t="s">
+        <v>354</v>
+      </c>
+      <c r="B73" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C73" s="78" t="s">
+        <v>296</v>
+      </c>
+      <c r="D73" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="E73" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73" s="78"/>
+      <c r="J73" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K73" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L73" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="62.15">
+      <c r="A74" t="s">
+        <v>355</v>
+      </c>
+      <c r="B74" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C74" s="78" t="s">
+        <v>298</v>
+      </c>
+      <c r="D74" s="78" t="s">
+        <v>299</v>
+      </c>
+      <c r="E74" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="F74" s="78"/>
+      <c r="J74" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K74" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L74" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="37.299999999999997">
+      <c r="A75" t="s">
+        <v>356</v>
+      </c>
+      <c r="B75" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C75" s="78" t="s">
+        <v>300</v>
+      </c>
+      <c r="D75" s="78" t="s">
+        <v>301</v>
+      </c>
+      <c r="E75" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="F75" s="78"/>
+      <c r="J75" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K75" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L75" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="37.299999999999997">
+      <c r="A76" t="s">
+        <v>357</v>
+      </c>
+      <c r="B76" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C76" s="78" t="s">
+        <v>302</v>
+      </c>
+      <c r="D76" s="78" t="s">
+        <v>303</v>
+      </c>
+      <c r="E76" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F76" s="78"/>
+      <c r="J76" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K76" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L76" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="49.75">
+      <c r="A77" t="s">
+        <v>358</v>
+      </c>
+      <c r="B77" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C77" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="D77" s="78" t="s">
+        <v>305</v>
+      </c>
+      <c r="E77" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F77" s="78"/>
+      <c r="J77" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K77" s="80" t="s">
+        <v>325</v>
+      </c>
+      <c r="L77" s="78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="62.15">
+      <c r="A78" t="s">
+        <v>359</v>
+      </c>
+      <c r="B78" s="77">
+        <v>44791</v>
+      </c>
+      <c r="C78" s="78" t="s">
+        <v>306</v>
+      </c>
+      <c r="D78" s="78" t="s">
+        <v>307</v>
+      </c>
+      <c r="E78" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="F78" s="78"/>
+      <c r="J78" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="K78" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="L78" s="78" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D38:D39"/>
     <mergeCell ref="I22:I23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
@@ -3246,31 +4758,65 @@
     <mergeCell ref="I28:I29"/>
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="K28:K29"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H35" r:id="rId1" display="http://email.com/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H35" r:id="rId1" display="http://email.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3278,19 +4824,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.4609375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1">
@@ -3505,33 +5051,33 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.2">
-      <c r="A17" s="65"/>
+    <row r="17" spans="1:6" ht="12.45">
+      <c r="A17" s="28"/>
       <c r="B17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-    </row>
-    <row r="18" spans="1:6" ht="66">
-      <c r="A18" s="65">
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+    </row>
+    <row r="18" spans="1:6" ht="62.15">
+      <c r="A18" s="28">
         <v>44779</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="E18" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="F18" s="66" t="s">
+      <c r="F18" s="29" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3634,63 +5180,63 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="66">
-      <c r="A28" s="65">
+    <row r="28" spans="1:6" ht="62.15">
+      <c r="A28" s="28">
         <v>44779</v>
       </c>
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="E28" s="66" t="s">
+      <c r="E28" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="F28" s="66" t="s">
+      <c r="F28" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="66">
-      <c r="A29" s="65">
+    <row r="29" spans="1:6" ht="37.299999999999997">
+      <c r="A29" s="28">
         <v>44779</v>
       </c>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="E29" s="66" t="s">
+      <c r="E29" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="F29" s="66" t="s">
+      <c r="F29" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="66">
-      <c r="A30" s="65">
+    <row r="30" spans="1:6" ht="62.15">
+      <c r="A30" s="28">
         <v>44779</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="E30" s="66" t="s">
+      <c r="E30" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="F30" s="66" t="s">
+      <c r="F30" s="29" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3701,7 +5247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3709,108 +5255,108 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45"/>
   <cols>
-    <col min="8" max="8" width="24.109375" customWidth="1"/>
+    <col min="8" max="8" width="24.07421875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="59" t="s">
+      <c r="H1" s="68"/>
+      <c r="I1" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="58" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="63"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="18" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="B3" s="57">
+      <c r="B3" s="62">
         <v>44784</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="63" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="64" t="s">
         <v>199</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="64" t="s">
         <v>198</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="64" t="s">
         <v>201</v>
       </c>
       <c r="G3" s="19">
@@ -3819,565 +5365,659 @@
       <c r="H3" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="50" t="s">
+      <c r="I3" s="65"/>
+      <c r="J3" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="66" t="s">
         <v>202</v>
       </c>
-      <c r="L3" s="50" t="s">
+      <c r="L3" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="M3" s="50" t="s">
+      <c r="M3" s="66" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="N3" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="50"/>
+      <c r="O3" s="66"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
       <c r="G4" s="19">
         <v>2</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="19">
         <v>3</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="19">
         <v>4</v>
       </c>
       <c r="H6" s="19"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="19">
         <v>5</v>
       </c>
       <c r="H7" s="19"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="51"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="64"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="47"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="51"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="56"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="47"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="48"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="49"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="73"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
+      <c r="A17" s="59"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="64"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="47"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="61"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="61"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="47"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="47"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="61"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="51"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="46"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="64"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
+      <c r="L28" s="61"/>
+      <c r="M28" s="61"/>
+      <c r="N28" s="61"/>
+      <c r="O28" s="61"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="47"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="61"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="61"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="48"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="59"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
+      <c r="A31" s="60"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="64"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="47"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
       <c r="G32" s="20"/>
       <c r="H32" s="21"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="47"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="47"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="61"/>
+      <c r="L33" s="61"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="61"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="48"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="59"/>
+      <c r="N34" s="59"/>
+      <c r="O34" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="118">
+    <mergeCell ref="O27:O30"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="K31:K34"/>
+    <mergeCell ref="L31:L34"/>
+    <mergeCell ref="M31:M34"/>
+    <mergeCell ref="K27:K30"/>
+    <mergeCell ref="L27:L30"/>
+    <mergeCell ref="M27:M30"/>
+    <mergeCell ref="N27:N30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="N22:N26"/>
+    <mergeCell ref="O22:O26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="K22:K26"/>
+    <mergeCell ref="L22:L26"/>
+    <mergeCell ref="M22:M26"/>
+    <mergeCell ref="N31:N34"/>
+    <mergeCell ref="O31:O34"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="M18:M21"/>
+    <mergeCell ref="N18:N21"/>
+    <mergeCell ref="O18:O21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="O8:O11"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="M8:M11"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="A3:A7"/>
@@ -4402,103 +6042,9 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="L3:L7"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="O8:O11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="M8:M11"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="O15:O17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="L18:L21"/>
-    <mergeCell ref="M18:M21"/>
-    <mergeCell ref="N18:N21"/>
-    <mergeCell ref="O18:O21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="N22:N26"/>
-    <mergeCell ref="O22:O26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="L22:L26"/>
-    <mergeCell ref="M22:M26"/>
-    <mergeCell ref="N31:N34"/>
-    <mergeCell ref="O31:O34"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="I31:I34"/>
-    <mergeCell ref="J31:J34"/>
-    <mergeCell ref="K31:K34"/>
-    <mergeCell ref="L31:L34"/>
-    <mergeCell ref="M31:M34"/>
-    <mergeCell ref="K27:K30"/>
-    <mergeCell ref="L27:L30"/>
-    <mergeCell ref="M27:M30"/>
-    <mergeCell ref="N27:N30"/>
-    <mergeCell ref="O27:O30"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="J3 J8 J12 J15 J18 J22 J27 J31" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="J3 J8 J12 J15 J18 J22 J27 J31">
       <formula1>"Reportado,En revisión,Finalizado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4508,18 +6054,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.69140625" customWidth="1"/>
+    <col min="4" max="4" width="17.23046875" customWidth="1"/>
+    <col min="6" max="6" width="24.4609375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>